<commit_message>
adding most up-to-date exfo test csvs and graphs
</commit_message>
<xml_diff>
--- a/Test Results - Second EXFO Group/switch_test_combined_EO193200515.xlsx
+++ b/Test Results - Second EXFO Group/switch_test_combined_EO193200515.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8F8D80-9325-4305-ABE3-E8A425FD064E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F0EC9-D61D-4B29-8A60-70A6DFDD6CEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="62520" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -992,7 +992,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2096,7 +2096,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3200,7 +3200,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4304,7 +4304,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -7504,7 +7504,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">

</xml_diff>